<commit_message>
alteração do codigo da planilha, não inseria na lista os autores
</commit_message>
<xml_diff>
--- a/php/src/WebScrapping/planilha.xlsx
+++ b/php/src/WebScrapping/planilha.xlsx
@@ -263,19 +263,39 @@
           <t>Bryan Nickson Santana Pinto</t>
         </is>
       </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+        </is>
+      </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Gabriella Almeida  Moura</t>
         </is>
       </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+        </is>
+      </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
           <t>Antonio Demuner</t>
         </is>
       </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+        </is>
+      </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
           <t>Elson Santiago Alvarenga</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
         </is>
       </c>
     </row>
@@ -300,6 +320,11 @@
           <t>Tiago   Bueno de Moraes</t>
         </is>
       </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Química  / Instituto de Ciências Exatas  / Universidade Federal de Minas Gerais</t>
+        </is>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="inlineStr">
@@ -322,14 +347,29 @@
           <t>Tatiana Monaretto</t>
         </is>
       </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Centre national de la recherche scientifique (CNRS)</t>
+        </is>
+      </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
           <t>Luiz Alberto Colnago</t>
         </is>
       </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>Empresa Brasileira de Pesquisa Agropecuária</t>
+        </is>
+      </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
           <t>Tiago   Bueno de Moraes</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Química  / Instituto de Ciências Exatas  / Universidade Federal de Minas Gerais</t>
         </is>
       </c>
     </row>
@@ -354,79 +394,159 @@
           <t>Katelyn Downey</t>
         </is>
       </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Sciences / Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
           <t>Bing Wu</t>
         </is>
       </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
           <t>Rudraksha Majumdar</t>
         </is>
       </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>Synex Medical</t>
+        </is>
+      </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
           <t>Daniel Lysak</t>
         </is>
       </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
           <t>Rajshree Ghosh Biswas</t>
         </is>
       </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="N5" s="2" t="inlineStr">
         <is>
           <t>Maryam  Tabatabaei-Anaraki</t>
         </is>
       </c>
+      <c r="O5" s="2" t="inlineStr">
+        <is>
+          <t>Chemistry / Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
           <t>Amy Jenne</t>
         </is>
       </c>
+      <c r="Q5" s="2" t="inlineStr">
+        <is>
+          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="R5" s="2" t="inlineStr">
         <is>
           <t>Xiang You</t>
         </is>
       </c>
+      <c r="S5" s="2" t="inlineStr">
+        <is>
+          <t>Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
       <c r="T5" s="2" t="inlineStr">
         <is>
           <t>Ronald Soong</t>
         </is>
       </c>
+      <c r="U5" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="V5" s="2" t="inlineStr">
         <is>
           <t>Daniel Lane</t>
         </is>
       </c>
+      <c r="W5" s="2" t="inlineStr">
+        <is>
+          <t>Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
       <c r="X5" s="2" t="inlineStr">
         <is>
           <t>Paul Helm</t>
         </is>
       </c>
+      <c r="Y5" s="2" t="inlineStr">
+        <is>
+          <t>Environmental Monitoring &amp; Reporting Branch / Ontario Ministry of the Environment</t>
+        </is>
+      </c>
       <c r="Z5" s="2" t="inlineStr">
         <is>
           <t>Anna Codina</t>
         </is>
       </c>
+      <c r="AA5" s="2" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
           <t>Venita Decker</t>
         </is>
       </c>
+      <c r="AC5" s="2" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
       <c r="AD5" s="2" t="inlineStr">
         <is>
           <t>Falko Busse</t>
         </is>
       </c>
+      <c r="AE5" s="2" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
       <c r="AF5" s="2" t="inlineStr">
         <is>
           <t>Myrna Simpson</t>
         </is>
       </c>
+      <c r="AG5" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Sciences / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="AH5" s="2" t="inlineStr">
         <is>
           <t>Andre Simpson</t>
+        </is>
+      </c>
+      <c r="AI5" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
         </is>
       </c>
     </row>
@@ -451,24 +571,49 @@
           <t>Banny S. B. Correia</t>
         </is>
       </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>Instituto de Química de São Carlos  / Universidade de São Paulo</t>
+        </is>
+      </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
           <t>Pollyana Ferreira da Silva Vianna</t>
         </is>
       </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>Instituto de Química de São Carlos  / Universidade de São Paulo</t>
+        </is>
+      </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
           <t>Caroline Ceribeli</t>
         </is>
       </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>Instituto de Química de São Carlos/ Universidade de São Paulo</t>
+        </is>
+      </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
           <t>Luiz Alberto Colnago</t>
         </is>
       </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>Empresa Brasileira de Pesquisa Agropecuária</t>
+        </is>
+      </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
           <t>Daniel Cardoso</t>
+        </is>
+      </c>
+      <c r="M6" s="2" t="inlineStr">
+        <is>
+          <t>Instituto de Química de São Carlos  / Universidade de São Paulo</t>
         </is>
       </c>
     </row>
@@ -493,14 +638,29 @@
           <t>Enya Silva de Oliveira</t>
         </is>
       </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry/Federal University of Goiás</t>
+        </is>
+      </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
           <t>Luciano Morais Lião</t>
         </is>
       </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry/Federal University of Goiás</t>
+        </is>
+      </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
           <t>Gerlon de Almeida Ribeiro Oliveira</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry/Federal University of Goiás</t>
         </is>
       </c>
     </row>
@@ -525,9 +685,19 @@
           <t>Amanda de Souza</t>
         </is>
       </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal dos Vales do Jequitinhonha e Mucuri</t>
+        </is>
+      </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
           <t>Rodrigo Verly</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal dos Vales do Jequitinhonha e Mucuri</t>
         </is>
       </c>
     </row>
@@ -552,29 +722,59 @@
           <t>Daniel Lysak</t>
         </is>
       </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
           <t>FLAVIO VINICIUS CRIZOSTOMO  KOCK</t>
         </is>
       </c>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
           <t>Salvatore Mamone</t>
         </is>
       </c>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>Biophysical Chemistry / Max Planck Institute / Max Planck Institute for Biophysical Chemistry</t>
+        </is>
+      </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
           <t>Stefan Glöggler</t>
         </is>
       </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>Biophysical Chemistry / Max Planck Institute / Max Planck Institute for Biophysical Chemistry</t>
+        </is>
+      </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
           <t>Ronald Soong</t>
         </is>
       </c>
+      <c r="M9" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="N9" s="2" t="inlineStr">
         <is>
           <t>Andre Simpson</t>
+        </is>
+      </c>
+      <c r="O9" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
         </is>
       </c>
     </row>
@@ -599,14 +799,29 @@
           <t>Kennedy  Daniel  de Carvalho Santos</t>
         </is>
       </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
           <t>Guilherme Dal Poggetto</t>
         </is>
       </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
           <t>Cláudio Francisco Tormena</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
         </is>
       </c>
     </row>
@@ -631,24 +846,49 @@
           <t>Gustavo  Solcia</t>
         </is>
       </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
           <t>Caio de Jesus Oliveira</t>
         </is>
       </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
       <c r="H11" s="2" t="inlineStr">
         <is>
           <t>Rafael Henrique Ferreira da Silva</t>
         </is>
       </c>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
           <t>Felipe Ferraz Derrico</t>
         </is>
       </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
           <t>Fernando Fernandes Paiva</t>
+        </is>
+      </c>
+      <c r="M11" s="2" t="inlineStr">
+        <is>
+          <t>Instituto de Física de São Carlos</t>
         </is>
       </c>
     </row>
@@ -673,19 +913,39 @@
           <t>Pedro Henrique Soares Cardoso</t>
         </is>
       </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Goiás</t>
+        </is>
+      </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
           <t>Luciano Morais Lião</t>
         </is>
       </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Goiás</t>
+        </is>
+      </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
           <t>Enya Silva de Oliveira</t>
         </is>
       </c>
+      <c r="I12" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry/Federal University of Goiás</t>
+        </is>
+      </c>
       <c r="J12" s="2" t="inlineStr">
         <is>
           <t>Gerlon de Almeida Ribeiro Oliveira</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>Instituto de Química / Universidade Federal de Goiás</t>
         </is>
       </c>
     </row>
@@ -710,14 +970,29 @@
           <t>Marília Vilela Salvador</t>
         </is>
       </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio Grande do Sul</t>
+        </is>
+      </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
           <t>Tiago  Venâncio</t>
         </is>
       </c>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
           <t>Francisco Paulo dos Santos</t>
+        </is>
+      </c>
+      <c r="I13" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio Grande do Sul</t>
         </is>
       </c>
     </row>
@@ -742,44 +1017,89 @@
           <t>Monica Bastawrous</t>
         </is>
       </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
           <t>Rajshree Ghosh Biswas</t>
         </is>
       </c>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="H14" s="2" t="inlineStr">
         <is>
           <t>Ronald Soong</t>
         </is>
       </c>
+      <c r="I14" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="J14" s="2" t="inlineStr">
         <is>
           <t>Sagar Wadhwa</t>
         </is>
       </c>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
           <t>Neil Mackinnon</t>
         </is>
       </c>
+      <c r="M14" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
       <c r="N14" s="2" t="inlineStr">
         <is>
           <t>Mazin Jouda</t>
         </is>
       </c>
+      <c r="O14" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
           <t>Dario Mager</t>
         </is>
       </c>
+      <c r="Q14" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
       <c r="R14" s="2" t="inlineStr">
         <is>
           <t>Jan Korvink</t>
         </is>
       </c>
+      <c r="S14" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
           <t>Andre Simpson</t>
+        </is>
+      </c>
+      <c r="U14" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
         </is>
       </c>
     </row>
@@ -804,39 +1124,79 @@
           <t>Yara Rocha</t>
         </is>
       </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
           <t>Victor U. Antunes</t>
         </is>
       </c>
+      <c r="G15" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
           <t>Yan  Ladeira</t>
         </is>
       </c>
+      <c r="I15" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Minas Gerais</t>
+        </is>
+      </c>
       <c r="J15" s="2" t="inlineStr">
         <is>
           <t>Adolfo Henrique de Moraes Silva</t>
         </is>
       </c>
+      <c r="K15" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Minas Gerais</t>
+        </is>
+      </c>
       <c r="L15" s="2" t="inlineStr">
         <is>
           <t>Renan Pirolla</t>
         </is>
       </c>
+      <c r="M15" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
       <c r="N15" s="2" t="inlineStr">
         <is>
           <t>Fábio Gozzo</t>
         </is>
       </c>
+      <c r="O15" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
           <t>Anthony  Mittermaier</t>
         </is>
       </c>
+      <c r="Q15" s="2" t="inlineStr">
+        <is>
+          <t>Department of Chemistry / McGill University / McGill University</t>
+        </is>
+      </c>
       <c r="R15" s="2" t="inlineStr">
         <is>
           <t>Denize  C. Favaro</t>
+        </is>
+      </c>
+      <c r="S15" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
         </is>
       </c>
     </row>
@@ -861,9 +1221,19 @@
           <t>Cassia  Chiari</t>
         </is>
       </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
           <t>Cláudio Francisco Tormena</t>
+        </is>
+      </c>
+      <c r="G16" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
         </is>
       </c>
     </row>
@@ -888,14 +1258,29 @@
           <t>Flávio Bueno dos Santos</t>
         </is>
       </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
           <t>Marcus Cardoso</t>
         </is>
       </c>
+      <c r="G17" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
           <t>Jose Rivera</t>
+        </is>
+      </c>
+      <c r="I17" s="2" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
         </is>
       </c>
     </row>
@@ -920,29 +1305,59 @@
           <t>Priscila  Rubim</t>
         </is>
       </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>Instituto Militar de Engenharia</t>
+        </is>
+      </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
           <t>Mychelle Monteiro</t>
         </is>
       </c>
+      <c r="G18" s="2" t="inlineStr">
+        <is>
+          <t>INCQS / Fundação Oswaldo Cruz</t>
+        </is>
+      </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
           <t>Filipe Soares Quirino da Silva</t>
         </is>
       </c>
+      <c r="I18" s="2" t="inlineStr">
+        <is>
+          <t>INCQS/Fiocruz</t>
+        </is>
+      </c>
       <c r="J18" s="2" t="inlineStr">
         <is>
           <t>Tanos Celmar Costa França</t>
         </is>
       </c>
+      <c r="K18" s="2" t="inlineStr">
+        <is>
+          <t>Instituto Militar de Engenharia</t>
+        </is>
+      </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
           <t>Joyce Sobreiro Francisco Diz de Almeida</t>
         </is>
       </c>
+      <c r="M18" s="2" t="inlineStr">
+        <is>
+          <t>Instituto Militar de Engenharia</t>
+        </is>
+      </c>
       <c r="N18" s="2" t="inlineStr">
         <is>
           <t>Jochen  Junker</t>
+        </is>
+      </c>
+      <c r="O18" s="2" t="inlineStr">
+        <is>
+          <t>CDTS / Presidência / Fundação Oswaldo Cruz</t>
         </is>
       </c>
     </row>
@@ -967,9 +1382,19 @@
           <t>Laiza  Bruzadelle Loureiro</t>
         </is>
       </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
       <c r="F19" s="2" t="inlineStr">
         <is>
           <t>Cláudio Francisco Tormena</t>
+        </is>
+      </c>
+      <c r="G19" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
         </is>
       </c>
     </row>
@@ -994,19 +1419,39 @@
           <t>Vinícius  Silva Pinto</t>
         </is>
       </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>Federal Institute Goiano</t>
+        </is>
+      </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
           <t>Christian Dias Gomides</t>
         </is>
       </c>
+      <c r="G20" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry, Federal University of Goias</t>
+        </is>
+      </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
           <t>Igor Flores</t>
         </is>
       </c>
+      <c r="I20" s="2" t="inlineStr">
+        <is>
+          <t>Federal Institute of Goiás</t>
+        </is>
+      </c>
       <c r="J20" s="2" t="inlineStr">
         <is>
           <t>Luciano Morais Lião</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry, Federal University of Goias</t>
         </is>
       </c>
     </row>
@@ -1031,19 +1476,39 @@
           <t>José Dias de Souza Filho</t>
         </is>
       </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
       <c r="F21" s="2" t="inlineStr">
         <is>
           <t>Jacqueline Souza</t>
         </is>
       </c>
+      <c r="G21" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
           <t>Marta de Lana</t>
         </is>
       </c>
+      <c r="I21" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
       <c r="J21" s="2" t="inlineStr">
         <is>
           <t>Gabriela Roberta Ramos Fernandes</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
         </is>
       </c>
     </row>
@@ -1068,24 +1533,49 @@
           <t>Beatriz Rosa  Penna</t>
         </is>
       </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>Instituto de Bioquímica Médica, Centro Nacional de Ressonância Magnética Nuclear Jiri Jonas, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
           <t>Thamires Moreira</t>
         </is>
       </c>
+      <c r="G22" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Bioquímica, Instituto de Química, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
           <t>Danielle Maria  Perpétua de Oliveira Santos</t>
         </is>
       </c>
+      <c r="I22" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Bioquímica, Instituto de Química, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="J22" s="2" t="inlineStr">
         <is>
           <t>Cristiane Dinis Ano Bom</t>
         </is>
       </c>
+      <c r="K22" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Bioquímica, Instituto de Química, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
           <t>Ana Paula Valente</t>
+        </is>
+      </c>
+      <c r="M22" s="2" t="inlineStr">
+        <is>
+          <t>Instituto de Bioquímica Médica, Centro Nacional de Ressonância Magnética Nuclear Jiri Jonas, Universidade Federal do Rio de Janeiro</t>
         </is>
       </c>
     </row>
@@ -1110,34 +1600,69 @@
           <t>Julie Lopes</t>
         </is>
       </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="F23" s="2" t="inlineStr">
         <is>
           <t>Beatriz Rosa  Penna</t>
         </is>
       </c>
+      <c r="G23" s="2" t="inlineStr">
+        <is>
+          <t>Instituto de Bioquímica Médica, Centro Nacional de Ressonância Magnética Nuclear Jiri Jonas, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="H23" s="2" t="inlineStr">
         <is>
           <t>Ana Paula Valente</t>
         </is>
       </c>
+      <c r="I23" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="J23" s="2" t="inlineStr">
         <is>
           <t>Leonardo  Bartkevihi</t>
         </is>
       </c>
+      <c r="K23" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
           <t>Paulo Antônio de Souza Mourão</t>
         </is>
       </c>
+      <c r="M23" s="2" t="inlineStr">
+        <is>
+          <t>Laboratório de Tecido Conjuntivo / Instituto de Bioquímica Médica / Universidade Federal de Juiz de Fora</t>
+        </is>
+      </c>
       <c r="N23" s="2" t="inlineStr">
         <is>
           <t>Francisco  Felipe  Bezerra</t>
         </is>
       </c>
+      <c r="O23" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Glicobiologia  / Bioquímica Médica / Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
           <t>Adriane Regina Todeschini</t>
+        </is>
+      </c>
+      <c r="Q23" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
         </is>
       </c>
     </row>
@@ -1162,19 +1687,39 @@
           <t>Elton Tadeu Montrazi</t>
         </is>
       </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>Department of Chemical and Biological Physics, Weizmann Institute of Science, Israel</t>
+        </is>
+      </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
           <t>Tatiana Monaretto</t>
         </is>
       </c>
+      <c r="G24" s="2" t="inlineStr">
+        <is>
+          <t>Centre National de La Recherche Scientifique, France</t>
+        </is>
+      </c>
       <c r="H24" s="2" t="inlineStr">
         <is>
           <t>Luiz Alberto Colnago</t>
         </is>
       </c>
+      <c r="I24" s="2" t="inlineStr">
+        <is>
+          <t>Embrapa Instrumentation, Brazil</t>
+        </is>
+      </c>
       <c r="J24" s="2" t="inlineStr">
         <is>
           <t>Tito José Bonagamba</t>
+        </is>
+      </c>
+      <c r="K24" s="2" t="inlineStr">
+        <is>
+          <t>São Carlos Institute of Physics, University of São Paulo, Brazil</t>
         </is>
       </c>
     </row>
@@ -1199,6 +1744,11 @@
           <t>Tatiana Monaretto</t>
         </is>
       </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>Centre national de la recherche scientifique (CNRS)</t>
+        </is>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="inlineStr">
@@ -1221,6 +1771,11 @@
           <t>Patrick Giraudeau</t>
         </is>
       </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>CEISAM / Faculté des Sciences et Techniques / Université de Nantes</t>
+        </is>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="inlineStr">
@@ -1243,6 +1798,11 @@
           <t>Andre Simpson</t>
         </is>
       </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="inlineStr">
@@ -1265,6 +1825,11 @@
           <t>Zeev Wiesman</t>
         </is>
       </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>LowField</t>
+        </is>
+      </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2" t="inlineStr">
@@ -1287,9 +1852,19 @@
           <t>Flavio Vinicius Crizostomo  Kock</t>
         </is>
       </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
           <t>Tiago Venâncio</t>
+        </is>
+      </c>
+      <c r="G29" s="2" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Universidade Federal de São Carlos</t>
         </is>
       </c>
     </row>
@@ -1314,6 +1889,11 @@
           <t>Juan Miguel López del Amo</t>
         </is>
       </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>NMR  / CIC energigune / CIC energigune</t>
+        </is>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="inlineStr">
@@ -1336,6 +1916,11 @@
           <t>Jeffrey Reimer</t>
         </is>
       </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>Dept Chem and BioM Engr / University of California</t>
+        </is>
+      </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="inlineStr">
@@ -1358,6 +1943,11 @@
           <t>Daniel Huster</t>
         </is>
       </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>University of Leipzig</t>
+        </is>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="inlineStr">
@@ -1380,6 +1970,11 @@
           <t>Pau Nolis</t>
         </is>
       </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>Universitat Autònoma de Barcelona</t>
+        </is>
+      </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="inlineStr">
@@ -1402,6 +1997,11 @@
           <t>Josep Saurí</t>
         </is>
       </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>NMR Research Scientist</t>
+        </is>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="inlineStr">
@@ -1424,6 +2024,11 @@
           <t>Gareth Morris</t>
         </is>
       </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>The University of Manchester</t>
+        </is>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="inlineStr">
@@ -1446,6 +2051,11 @@
           <t>Antonio Gilberto Ferreira</t>
         </is>
       </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="inlineStr">
@@ -1468,6 +2078,11 @@
           <t>Scott Prosser</t>
         </is>
       </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="2" t="inlineStr">
@@ -1490,14 +2105,29 @@
           <t> Jeremy Good</t>
         </is>
       </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>London, UK / Cryogenic Ltd</t>
+        </is>
+      </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
           <t>Eugeny Kryukov</t>
         </is>
       </c>
+      <c r="G38" s="2" t="inlineStr">
+        <is>
+          <t>Cryogenic Ltd</t>
+        </is>
+      </c>
       <c r="H38" s="2" t="inlineStr">
         <is>
           <t>Dr. Stephen Burgess</t>
+        </is>
+      </c>
+      <c r="I38" s="2" t="inlineStr">
+        <is>
+          <t>Cryogenic Ltd</t>
         </is>
       </c>
     </row>
@@ -1522,6 +2152,11 @@
           <t>Giselle de Araujo Lima e Souza</t>
         </is>
       </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+        </is>
+      </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="inlineStr">
@@ -1544,6 +2179,11 @@
           <t>Ariel Sarotti</t>
         </is>
       </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>Chimica / Chimica / Universidad Nacional de Rosario</t>
+        </is>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2" t="inlineStr">
@@ -1566,9 +2206,19 @@
           <t>Sophia Hayes</t>
         </is>
       </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>Chemistry / Arts &amp; Sciences / Washington University in St. Louis</t>
+        </is>
+      </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
           <t>He Sun</t>
+        </is>
+      </c>
+      <c r="G41" s="2" t="inlineStr">
+        <is>
+          <t>Chemistry / Arts &amp; Sciences / Washington University in St. Louis</t>
         </is>
       </c>
     </row>
@@ -1593,6 +2243,11 @@
           <t>Jair Freitas</t>
         </is>
       </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Espírito Santo, Brazil</t>
+        </is>
+      </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="inlineStr">
@@ -1615,6 +2270,11 @@
           <t>Toshikazu Miyoshi</t>
         </is>
       </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>The University of Akron</t>
+        </is>
+      </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="inlineStr">
@@ -1637,6 +2297,11 @@
           <t>Marek Pruski</t>
         </is>
       </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>Iowa State University</t>
+        </is>
+      </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="inlineStr">
@@ -1659,6 +2324,11 @@
           <t>Yushan Wei</t>
         </is>
       </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>Niumag</t>
+        </is>
+      </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="inlineStr">
@@ -1681,6 +2351,11 @@
           <t>Juan Araneda</t>
         </is>
       </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>Nanalysis Corp.</t>
+        </is>
+      </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="inlineStr">
@@ -1703,6 +2378,11 @@
           <t>Clemens Anklin</t>
         </is>
       </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="2" t="inlineStr">
@@ -1725,14 +2405,29 @@
           <t>Søren Balling Engelsen</t>
         </is>
       </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>University of Copenhagen</t>
+        </is>
+      </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
           <t>Bekzod  Khakimov </t>
         </is>
       </c>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>University of Copenhagen</t>
+        </is>
+      </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
           <t>Viola  Aru</t>
+        </is>
+      </c>
+      <c r="I48" s="2" t="inlineStr">
+        <is>
+          <t>University of Copenhagen</t>
         </is>
       </c>
     </row>
@@ -1757,6 +2452,11 @@
           <t>Felipe Simoes</t>
         </is>
       </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>Hélio para Ressonancia Magnética / Hélio para Ressonancia Magnética / Air Products do Brasil Ltda</t>
+        </is>
+      </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="inlineStr">
@@ -1779,6 +2479,11 @@
           <t>Marcel Lachenmann</t>
         </is>
       </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>Oxford Instruments</t>
+        </is>
+      </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="inlineStr">
@@ -1801,6 +2506,11 @@
           <t>Hector Robert</t>
         </is>
       </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>Magritek, Inc</t>
+        </is>
+      </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="inlineStr">
@@ -1823,6 +2533,11 @@
           <t>Marcus Vinícius Cangussu Cardoso</t>
         </is>
       </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="inlineStr">
@@ -1845,6 +2560,11 @@
           <t>Annick Moing</t>
         </is>
       </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>INRAE Bordeaux, France</t>
+        </is>
+      </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="2" t="inlineStr">
@@ -1867,24 +2587,49 @@
           <t>Igor d'Anciães Almeida Silva</t>
         </is>
       </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
           <t>Hellmut Eckert</t>
         </is>
       </c>
+      <c r="G54" s="2" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
       <c r="H54" s="2" t="inlineStr">
         <is>
           <t>Ana Candida Martins Rodrigues</t>
         </is>
       </c>
+      <c r="I54" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
       <c r="J54" s="2" t="inlineStr">
         <is>
           <t>Adraiana Nieto-Munoz</t>
         </is>
       </c>
+      <c r="K54" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
       <c r="L54" s="2" t="inlineStr">
         <is>
           <t>Vinicius Zallocco</t>
+        </is>
+      </c>
+      <c r="M54" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
         </is>
       </c>
     </row>
@@ -1909,6 +2654,11 @@
           <t>Esteban Anoardo</t>
         </is>
       </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>Laboratorio de Relaxometría y Técnicas Especiales (LaRTE). / Instituto de Física Enrique Gaviola, CONICET. Córdoba, Argentina. / FaMAF - Universidad Nacional de Córdoba. Córdoba, Argentina.</t>
+        </is>
+      </c>
     </row>
     <row r="56" spans="1:39">
       <c r="A56" s="2" t="inlineStr">
@@ -1931,89 +2681,179 @@
           <t>Amy Jenne</t>
         </is>
       </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
           <t>Sebastian Von Der Ecken</t>
         </is>
       </c>
+      <c r="G56" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
       <c r="H56" s="2" t="inlineStr">
         <is>
           <t>Vincent Moxley-Paquette</t>
         </is>
       </c>
+      <c r="I56" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="J56" s="2" t="inlineStr">
         <is>
           <t>Ian Swyer</t>
         </is>
       </c>
+      <c r="K56" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
       <c r="L56" s="2" t="inlineStr">
         <is>
           <t>Ronald Soong</t>
         </is>
       </c>
+      <c r="M56" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="N56" s="2" t="inlineStr">
         <is>
           <t>Monica Bastawrous</t>
         </is>
       </c>
+      <c r="O56" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
       <c r="P56" s="2" t="inlineStr">
         <is>
           <t>Falko Busse</t>
         </is>
       </c>
+      <c r="Q56" s="2" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
       <c r="R56" s="2" t="inlineStr">
         <is>
           <t>Wolfgang Bermel</t>
         </is>
       </c>
+      <c r="S56" s="2" t="inlineStr">
+        <is>
+          <t>Biospin GmbH / BRUKER</t>
+        </is>
+      </c>
       <c r="T56" s="2" t="inlineStr">
         <is>
           <t>Daniel Schmidig</t>
         </is>
       </c>
+      <c r="U56" s="2" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
       <c r="V56" s="2" t="inlineStr">
         <is>
           <t>Till Kuehn</t>
         </is>
       </c>
+      <c r="W56" s="2" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
       <c r="X56" s="2" t="inlineStr">
         <is>
           <t>Rainer Kuemmerle</t>
         </is>
       </c>
+      <c r="Y56" s="2" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
       <c r="Z56" s="2" t="inlineStr">
         <is>
           <t>Danijela Al Adwan-Stojilkovic</t>
         </is>
       </c>
+      <c r="AA56" s="2" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
       <c r="AB56" s="2" t="inlineStr">
         <is>
           <t>Stephan Graf</t>
         </is>
       </c>
+      <c r="AC56" s="2" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
       <c r="AD56" s="2" t="inlineStr">
         <is>
           <t>Thomas Frei</t>
         </is>
       </c>
+      <c r="AE56" s="2" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
       <c r="AF56" s="2" t="inlineStr">
         <is>
           <t>Martine Monette</t>
         </is>
       </c>
+      <c r="AG56" s="2" t="inlineStr">
+        <is>
+          <t>Canada Ltd / BRUKER</t>
+        </is>
+      </c>
       <c r="AH56" s="2" t="inlineStr">
         <is>
           <t>Henry Stronks</t>
         </is>
       </c>
+      <c r="AI56" s="2" t="inlineStr">
+        <is>
+          <t>Canada Ltd / BRUKER</t>
+        </is>
+      </c>
       <c r="AJ56" s="2" t="inlineStr">
         <is>
           <t>Aaron Wheeler</t>
         </is>
       </c>
+      <c r="AK56" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
       <c r="AL56" s="2" t="inlineStr">
         <is>
           <t>Andre Simpson</t>
+        </is>
+      </c>
+      <c r="AM56" s="2" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
         </is>
       </c>
     </row>
@@ -2038,64 +2878,129 @@
           <t>Rajshree Ghosh Biswas</t>
         </is>
       </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="F57" s="2" t="inlineStr">
         <is>
           <t>Ronald Soong</t>
         </is>
       </c>
+      <c r="G57" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
           <t>Paris Ning</t>
         </is>
       </c>
+      <c r="I57" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="J57" s="2" t="inlineStr">
         <is>
           <t>Daniel Lane</t>
         </is>
       </c>
+      <c r="K57" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="L57" s="2" t="inlineStr">
         <is>
           <t>Daniel Schmidig</t>
         </is>
       </c>
+      <c r="M57" s="2" t="inlineStr">
+        <is>
+          <t>Biospin AG / Bruker</t>
+        </is>
+      </c>
       <c r="N57" s="2" t="inlineStr">
         <is>
           <t>Peter de Castro</t>
         </is>
       </c>
+      <c r="O57" s="2" t="inlineStr">
+        <is>
+          <t>Biospin AG / Bruker</t>
+        </is>
+      </c>
       <c r="P57" s="2" t="inlineStr">
         <is>
           <t>Stephan Graf</t>
         </is>
       </c>
+      <c r="Q57" s="2" t="inlineStr">
+        <is>
+          <t>Biospin AG / Bruker</t>
+        </is>
+      </c>
       <c r="R57" s="2" t="inlineStr">
         <is>
           <t>Sebastian Wegner</t>
         </is>
       </c>
+      <c r="S57" s="2" t="inlineStr">
+        <is>
+          <t>Bruker Biospin GmbH / Bruker</t>
+        </is>
+      </c>
       <c r="T57" s="2" t="inlineStr">
         <is>
           <t>Falko Busse</t>
         </is>
       </c>
+      <c r="U57" s="2" t="inlineStr">
+        <is>
+          <t>Bruker Biospin GmbH / Bruker</t>
+        </is>
+      </c>
       <c r="V57" s="2" t="inlineStr">
         <is>
           <t>Jochem Struppe</t>
         </is>
       </c>
+      <c r="W57" s="2" t="inlineStr">
+        <is>
+          <t>Bruker BioSpin</t>
+        </is>
+      </c>
       <c r="X57" s="2" t="inlineStr">
         <is>
           <t>Michael  Fey</t>
         </is>
       </c>
+      <c r="Y57" s="2" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
       <c r="Z57" s="2" t="inlineStr">
         <is>
           <t>Myrna Simpson</t>
         </is>
       </c>
+      <c r="AA57" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
       <c r="AB57" s="2" t="inlineStr">
         <is>
           <t>Andre Simpson</t>
+        </is>
+      </c>
+      <c r="AC57" s="2" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
         </is>
       </c>
     </row>
@@ -2120,29 +3025,59 @@
           <t>VANESSA BEZERRA DE OLIVEIRA LEITE</t>
         </is>
       </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Estado do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
           <t>Talita Stelling De Araujo</t>
         </is>
       </c>
+      <c r="G58" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
           <t>Rafael Alves de Andrade</t>
         </is>
       </c>
+      <c r="I58" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="J58" s="2" t="inlineStr">
         <is>
           <t>Fabio C. L. Almeida</t>
         </is>
       </c>
+      <c r="K58" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="L58" s="2" t="inlineStr">
         <is>
           <t>Marcius da Silva Almeida</t>
         </is>
       </c>
+      <c r="M58" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
       <c r="N58" s="2" t="inlineStr">
         <is>
           <t>Claudia Jorge do Nascimento</t>
+        </is>
+      </c>
+      <c r="O58" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Estado do Rio de Janeiro</t>
         </is>
       </c>
     </row>
@@ -2167,6 +3102,11 @@
           <t>Fabio Ceneviva  Lacerda Almeida</t>
         </is>
       </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="2" t="inlineStr">
@@ -2189,6 +3129,11 @@
           <t>Clemens  Anklin</t>
         </is>
       </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>NMR Applicaitons / Bruker Biospin</t>
+        </is>
+      </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="2" t="inlineStr">
@@ -2211,6 +3156,11 @@
           <t>Julien Orts</t>
         </is>
       </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>Department of Pharmaceutical Sciences / Faculty of Life Sciences / University of Vienna</t>
+        </is>
+      </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="2" t="inlineStr">
@@ -2233,6 +3183,11 @@
           <t>Donald Bouchard</t>
         </is>
       </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>Alegre Science Inc</t>
+        </is>
+      </c>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="2" t="inlineStr">
@@ -2255,24 +3210,49 @@
           <t>Giselle de Araujo Lima e Souza</t>
         </is>
       </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+        </is>
+      </c>
       <c r="F63" s="2" t="inlineStr">
         <is>
           <t>Maria Enrica Di Pietro</t>
         </is>
       </c>
+      <c r="G63" s="2" t="inlineStr">
+        <is>
+          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+        </is>
+      </c>
       <c r="H63" s="2" t="inlineStr">
         <is>
           <t>Giovanni Battista Appetecchi</t>
         </is>
       </c>
+      <c r="I63" s="2" t="inlineStr">
+        <is>
+          <t>Department for Sustainability (SSPT) / Italian National Agency for New Technologies, Energy and Sustainable Economic Development / ENEA</t>
+        </is>
+      </c>
       <c r="J63" s="2" t="inlineStr">
         <is>
           <t>Patricia Fazzio Martinez</t>
         </is>
       </c>
+      <c r="K63" s="2" t="inlineStr">
+        <is>
+          <t>School of Chemical Engineering/ University of Campinas/ Campinas/ Brazil</t>
+        </is>
+      </c>
       <c r="L63" s="2" t="inlineStr">
         <is>
           <t>Andrea Mele</t>
+        </is>
+      </c>
+      <c r="M63" s="2" t="inlineStr">
+        <is>
+          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
         </is>
       </c>
     </row>

</xml_diff>